<commit_message>
Deploying to gh-pages from  @ 996dd361e35b63b5d4fa8205cd78bf8e816f3327 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/4.1.2.xlsx
+++ b/en/downloads/data-excel/4.1.2.xlsx
@@ -346,27 +346,15 @@
     <t>4.1.2 Completion rate (primary education, lower secondary education, upper secondary education)</t>
   </si>
   <si>
-    <t>4.1.2 Бүтүрүү коэффициенти (башталгыч билим берүү, толук эмес жана жогорку орто билим берүү)</t>
-  </si>
-  <si>
-    <t>Башталгыч билим берүүнү аяктоо көрсөткүчү</t>
-  </si>
-  <si>
     <t>Primary education completion rate</t>
   </si>
   <si>
-    <t>Толук эмес орто билим берүүнүн көрсөткүчү</t>
-  </si>
-  <si>
     <t>Lower Secondary Education Completion Rate</t>
   </si>
   <si>
     <t>Secondary education completion rate</t>
   </si>
   <si>
-    <t>Толук орто билим берүүнүн бүтүрүү коэффициенти</t>
-  </si>
-  <si>
     <t>(пайыз менен)</t>
   </si>
   <si>
@@ -383,6 +371,18 @@
   </si>
   <si>
     <t>According to the Multiple Indicator Cluster Survey, 2018, 2023</t>
+  </si>
+  <si>
+    <t>4.1.2 Бүтүрүүнүн пайызы (башталгыч билим берүү, толук эмес жана жогорку орто билим берүү)</t>
+  </si>
+  <si>
+    <t>Башталгыч билим берүүнү аяктоо пайызы</t>
+  </si>
+  <si>
+    <t>Толук эмес орто билим берүүнү аяктоо пайызы</t>
+  </si>
+  <si>
+    <t>Толук орто билим берүүнү аяктоо пайызы</t>
   </si>
 </sst>
 </file>
@@ -979,7 +979,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>92</v>
@@ -993,13 +993,13 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1033,13 +1033,13 @@
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>93</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D5" s="25">
         <v>99.2</v>
@@ -1593,13 +1593,13 @@
     </row>
     <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B38" s="26" t="s">
         <v>94</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D38" s="25">
         <v>98.9</v>
@@ -1971,13 +1971,13 @@
     </row>
     <row r="61" spans="1:5" s="29" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="26" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B61" s="26" t="s">
         <v>95</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D61" s="30">
         <v>86.8</v>
@@ -2349,13 +2349,13 @@
     </row>
     <row r="84" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A84" s="37" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B84" s="37" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C84" s="37" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>